<commit_message>
Test for shifted QR 3x3
</commit_message>
<xml_diff>
--- a/jacobi/src/test/resources/jacobi/test/data/ShiftedQR3x3Test.xlsx
+++ b/jacobi/src/test/resources/jacobi/test/data/ShiftedQR3x3Test.xlsx
@@ -4,21 +4,23 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="3"/>
+    <workbookView xWindow="-180" yWindow="0" windowWidth="27795" windowHeight="12450" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="eig-test-1" sheetId="1" r:id="rId1"/>
     <sheet name="eig-test-2" sheetId="2" r:id="rId2"/>
     <sheet name="eig-test-3" sheetId="4" r:id="rId3"/>
     <sheet name="eig-test-4" sheetId="5" r:id="rId4"/>
-    <sheet name="rand" sheetId="3" r:id="rId5"/>
+    <sheet name="step-test-1" sheetId="6" r:id="rId5"/>
+    <sheet name="step-test-2" sheetId="7" r:id="rId6"/>
+    <sheet name="rand" sheetId="3" r:id="rId7"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="42">
   <si>
     <t>#1</t>
   </si>
@@ -152,12 +154,31 @@
   <si>
     <t>ae+ak+ek-jf-bd=</t>
   </si>
+  <si>
+    <t>r=</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c=</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s=</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -914,7 +935,7 @@
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f t="shared" ref="A15:C15" si="2">A5</f>
+        <f t="shared" ref="A15:B15" si="2">A5</f>
         <v>0</v>
       </c>
       <c r="B15">
@@ -2184,8 +2205,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3:R22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2739,10 +2760,1612 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AG32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:C32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0.92249981064206388</v>
+      </c>
+      <c r="B3">
+        <v>6.0073509615214959E-2</v>
+      </c>
+      <c r="C3">
+        <v>-5.2281770299375747</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <f>A3</f>
+        <v>0.92249981064206388</v>
+      </c>
+      <c r="H3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3">
+        <f>F3+F7+F10</f>
+        <v>-11.924979476360399</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" s="1">
+        <f>R9</f>
+        <v>-24.086621133178244</v>
+      </c>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1">
+        <f>L3/3</f>
+        <v>-8.0288737110594148</v>
+      </c>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R3" s="1">
+        <f>-I3</f>
+        <v>11.924979476360399</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>-3.8428342895633278</v>
+      </c>
+      <c r="B4">
+        <v>-6.0431420652927192</v>
+      </c>
+      <c r="C4">
+        <v>8.9018925090847958</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <f>B3</f>
+        <v>6.0073509615214959E-2</v>
+      </c>
+      <c r="H4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I4">
+        <f>F3*F7+F3*F10+F7*F10-F9*F8-F4*F6</f>
+        <v>23.31509070402733</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" s="1">
+        <f>R10</f>
+        <v>-11.676561209538889</v>
+      </c>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1">
+        <f>L4/2</f>
+        <v>-5.8382806047694444</v>
+      </c>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R4" s="1">
+        <f>I4</f>
+        <v>23.31509070402733</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>0.69463219352170036</v>
+      </c>
+      <c r="C5">
+        <v>-6.8043372217097442</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <f>C3</f>
+        <v>-5.2281770299375747</v>
+      </c>
+      <c r="H5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5">
+        <f>F3*F7*F10+F5*F6*F9-F3*F9*F8-F4*F6*F10</f>
+        <v>44.613555342986842</v>
+      </c>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R5" s="1">
+        <f>-I5</f>
+        <v>-44.613555342986842</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <f>A4</f>
+        <v>-3.8428342895633278</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L6" s="1">
+        <f>-L4/2</f>
+        <v>5.8382806047694444</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N6" s="1">
+        <f>L4*L4/4 + L3*L3*L3/27</f>
+        <v>-483.47826476370739</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <f>B4</f>
+        <v>-6.0431420652927192</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L7" s="1">
+        <f>L6</f>
+        <v>5.8382806047694444</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N7" s="1">
+        <f>N6</f>
+        <v>-483.47826476370739</v>
+      </c>
+      <c r="O7" s="1" t="str">
+        <f>O6</f>
+        <v>)</v>
+      </c>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R7" s="1">
+        <f>-R3/3</f>
+        <v>-3.9749931587867997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8">
+        <f>C4</f>
+        <v>8.9018925090847958</v>
+      </c>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9">
+        <f>B5</f>
+        <v>0.69463219352170036</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L9" s="1" t="e">
+        <f>POWER(L6+SQRT(N6), 1/3)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R9" s="1">
+        <f>3*R7*R7+2*R3*R7+R4</f>
+        <v>-24.086621133178244</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10">
+        <f>C5</f>
+        <v>-6.8043372217097442</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L10" s="1" t="e">
+        <f>POWER(L7-SQRT(N7), 1/3)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R10" s="1">
+        <f>R7*R7*R7+R3*R7*R7+R4*R7+R5</f>
+        <v>-11.676561209538889</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L12" s="1" t="e">
+        <f>L9+L10</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="R12" s="1" t="e">
+        <f>L12+R7</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1" t="e">
+        <f>L12*L12*L12+L3*L12+L4</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L16" s="1">
+        <f>SQRT(L6*L6+ABS(N6))</f>
+        <v>22.750028245778829</v>
+      </c>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O16" s="1">
+        <f>SQRT(-L3/3)</f>
+        <v>2.8335267267240334</v>
+      </c>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+    </row>
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="K17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L17" s="1">
+        <f>SQRT(-N6)/L6</f>
+        <v>3.7662011595985159</v>
+      </c>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+    </row>
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="K18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L18" s="1">
+        <f>ATAN(L17)</f>
+        <v>1.311265209326725</v>
+      </c>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+    </row>
+    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="K19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L19" s="1">
+        <f>COS(L18/3)</f>
+        <v>0.90598799052345402</v>
+      </c>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+    </row>
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+    </row>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="K21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L21" s="1">
+        <f>2*O16*L19</f>
+        <v>5.1342823704784148</v>
+      </c>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+    </row>
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="K22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L22" s="1">
+        <f>SIGN(-L4/(L21*L21+L3))*ABS(L21)</f>
+        <v>5.1342823704784148</v>
+      </c>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="R22" s="1">
+        <f>L22+R7</f>
+        <v>1.1592892116916151</v>
+      </c>
+    </row>
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f>A3-R22</f>
+        <v>-0.23678940104955126</v>
+      </c>
+      <c r="B24">
+        <f t="shared" ref="B24:C24" si="0">B3</f>
+        <v>6.0073509615214959E-2</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>-5.2281770299375747</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F24" s="1">
+        <f>SQRT(A24*A24+A25*A25)</f>
+        <v>3.8501226730447295</v>
+      </c>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1">
+        <f>F25</f>
+        <v>-6.1501780893203323E-2</v>
+      </c>
+      <c r="I24" s="1">
+        <f>-F26</f>
+        <v>-0.99810697369919443</v>
+      </c>
+      <c r="J24" s="1">
+        <v>0</v>
+      </c>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1">
+        <f t="array" ref="L24:N26">MMULT(H24:J26,A24:C26)</f>
+        <v>3.8501226730447291</v>
+      </c>
+      <c r="M24" s="1">
+        <v>7.1851022573214181</v>
+      </c>
+      <c r="N24" s="1">
+        <v>-8.5634987942720553</v>
+      </c>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q24" s="1">
+        <f>SQRT(M25*M25+M26*M26)</f>
+        <v>0.85758064480905549</v>
+      </c>
+      <c r="R24" s="1"/>
+      <c r="S24" s="1">
+        <v>1</v>
+      </c>
+      <c r="T24" s="1">
+        <v>0</v>
+      </c>
+      <c r="U24" s="1">
+        <v>0</v>
+      </c>
+      <c r="V24" s="1"/>
+      <c r="W24" s="1">
+        <f t="array" ref="W24:Y26">MMULT(S24:U26,L24:N26)</f>
+        <v>3.8501226730447291</v>
+      </c>
+      <c r="X24" s="1">
+        <v>7.1851022573214181</v>
+      </c>
+      <c r="Y24" s="1">
+        <v>-8.5634987942720553</v>
+      </c>
+      <c r="Z24" s="1"/>
+      <c r="AA24" s="1">
+        <f t="array" ref="AA24:AC26">MMULT(W24:Y26,TRANSPOSE(H24:J26))</f>
+        <v>-7.4082900708238819</v>
+      </c>
+      <c r="AB24" s="1">
+        <v>3.4009377048382849</v>
+      </c>
+      <c r="AC24" s="1">
+        <v>-8.5634987942720553</v>
+      </c>
+      <c r="AE24" s="1">
+        <f t="array" ref="AE24:AG26">MMULT(AA24:AC26,TRANSPOSE(S24:U26))</f>
+        <v>-7.4082900708238819</v>
+      </c>
+      <c r="AF24" s="1">
+        <v>-4.9418968485516066</v>
+      </c>
+      <c r="AG24" s="1">
+        <v>-7.7767309590833449</v>
+      </c>
+    </row>
+    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f t="shared" ref="A25:C25" si="1">A4</f>
+        <v>-3.8428342895633278</v>
+      </c>
+      <c r="B25">
+        <f>B4-R22</f>
+        <v>-7.2024312769843348</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="1"/>
+        <v>8.9018925090847958</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F25" s="1">
+        <f>A24/F24</f>
+        <v>-6.1501780893203323E-2</v>
+      </c>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1">
+        <f>F26</f>
+        <v>0.99810697369919443</v>
+      </c>
+      <c r="I25" s="1">
+        <f>F25</f>
+        <v>-6.1501780893203323E-2</v>
+      </c>
+      <c r="J25" s="1">
+        <v>0</v>
+      </c>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1">
+        <v>-2.7755575615628914E-17</v>
+      </c>
+      <c r="M25" s="1">
+        <v>0.50292213917697681</v>
+      </c>
+      <c r="N25" s="1">
+        <v>-5.7657621959432159</v>
+      </c>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q25" s="1">
+        <f>M25/Q24</f>
+        <v>0.58644296862478151</v>
+      </c>
+      <c r="R25" s="1"/>
+      <c r="S25" s="1">
+        <v>0</v>
+      </c>
+      <c r="T25" s="1">
+        <f>Q25</f>
+        <v>0.58644296862478151</v>
+      </c>
+      <c r="U25" s="1">
+        <f>-Q26</f>
+        <v>0.80999052127204152</v>
+      </c>
+      <c r="V25" s="1"/>
+      <c r="W25" s="1">
+        <v>-1.6277062159919018E-17</v>
+      </c>
+      <c r="X25" s="1">
+        <v>0.85758064480905549</v>
+      </c>
+      <c r="Y25" s="1">
+        <v>-9.8317526245800533</v>
+      </c>
+      <c r="Z25" s="1"/>
+      <c r="AA25" s="1">
+        <v>-0.85595722209337011</v>
+      </c>
+      <c r="AB25" s="1">
+        <v>-5.2742736915298571E-2</v>
+      </c>
+      <c r="AC25" s="1">
+        <v>-9.8317526245800533</v>
+      </c>
+      <c r="AE25" s="1">
+        <v>-0.85595722209337011</v>
+      </c>
+      <c r="AF25" s="1">
+        <v>-7.9945570406113635</v>
+      </c>
+      <c r="AG25" s="1">
+        <v>-5.7230410789758768</v>
+      </c>
+    </row>
+    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f t="shared" ref="A26:B26" si="2">A5</f>
+        <v>0</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="2"/>
+        <v>0.69463219352170036</v>
+      </c>
+      <c r="C26">
+        <f>C5-R22</f>
+        <v>-7.9636264334013589</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F26" s="1">
+        <f>-A25/F24</f>
+        <v>0.99810697369919443</v>
+      </c>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1">
+        <v>0</v>
+      </c>
+      <c r="I26" s="1">
+        <v>0</v>
+      </c>
+      <c r="J26" s="1">
+        <v>1</v>
+      </c>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1">
+        <v>0</v>
+      </c>
+      <c r="M26" s="1">
+        <v>0.69463219352170036</v>
+      </c>
+      <c r="N26" s="1">
+        <v>-7.9636264334013589</v>
+      </c>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q26" s="1">
+        <f>-M26/Q24</f>
+        <v>-0.80999052127204152</v>
+      </c>
+      <c r="R26" s="1"/>
+      <c r="S26" s="1">
+        <v>0</v>
+      </c>
+      <c r="T26" s="1">
+        <f>Q26</f>
+        <v>-0.80999052127204152</v>
+      </c>
+      <c r="U26" s="1">
+        <f>Q25</f>
+        <v>0.58644296862478151</v>
+      </c>
+      <c r="V26" s="1"/>
+      <c r="W26" s="1">
+        <v>2.2481753161108828E-17</v>
+      </c>
+      <c r="X26" s="1">
+        <v>5.5511151231257827E-17</v>
+      </c>
+      <c r="Y26" s="1">
+        <v>2.6645352591003757E-15</v>
+      </c>
+      <c r="Z26" s="1"/>
+      <c r="AA26" s="1">
+        <v>-5.6788735018998655E-17</v>
+      </c>
+      <c r="AB26" s="1">
+        <v>1.9025159950932341E-17</v>
+      </c>
+      <c r="AC26" s="1">
+        <v>2.6645352591003757E-15</v>
+      </c>
+      <c r="AE26" s="1">
+        <v>-5.6788735018998655E-17</v>
+      </c>
+      <c r="AF26" s="1">
+        <v>2.1694054747466336E-15</v>
+      </c>
+      <c r="AG26" s="1">
+        <v>1.547187768126286E-15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>3</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <f>AE24+R22</f>
+        <v>-6.2490008591322663</v>
+      </c>
+      <c r="B30">
+        <f t="shared" ref="B30:C30" si="3">AF24</f>
+        <v>-4.9418968485516066</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="3"/>
+        <v>-7.7767309590833449</v>
+      </c>
+    </row>
+    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <f t="shared" ref="A31:A32" si="4">AE25</f>
+        <v>-0.85595722209337011</v>
+      </c>
+      <c r="B31">
+        <f>AF25+R22</f>
+        <v>-6.8352678289197488</v>
+      </c>
+      <c r="C31">
+        <f t="shared" ref="C31:C32" si="5">AG25</f>
+        <v>-5.7230410789758768</v>
+      </c>
+    </row>
+    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <f t="shared" si="4"/>
+        <v>-5.6788735018998655E-17</v>
+      </c>
+      <c r="B32">
+        <f t="shared" ref="B31:B32" si="6">AF26</f>
+        <v>2.1694054747466336E-15</v>
+      </c>
+      <c r="C32">
+        <f>AG26+R22</f>
+        <v>1.1592892116916167</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AG32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:C32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>-5.8070870276298852</v>
+      </c>
+      <c r="B3">
+        <v>7.1044250520173655</v>
+      </c>
+      <c r="C3">
+        <v>-7.3708461838257655</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <f>A3</f>
+        <v>-5.8070870276298852</v>
+      </c>
+      <c r="H3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3">
+        <f>F3+F7+F10</f>
+        <v>-0.37269246979397685</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" s="1">
+        <f>R9</f>
+        <v>-12.587711452786484</v>
+      </c>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1">
+        <f>L3/3</f>
+        <v>-4.1959038175954948</v>
+      </c>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R3" s="1">
+        <f>-I3</f>
+        <v>0.37269246979397685</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>-1.7283573982055174</v>
+      </c>
+      <c r="B4">
+        <v>-4.0710190005233819</v>
+      </c>
+      <c r="C4">
+        <v>6.9729152225895739</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <f>B3</f>
+        <v>7.1044250520173655</v>
+      </c>
+      <c r="H4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I4">
+        <f>F3*F7+F3*F10+F7*F10-F9*F8-F4*F6</f>
+        <v>-12.541411560439439</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" s="1">
+        <f>R10</f>
+        <v>6.9790088341374332</v>
+      </c>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1">
+        <f>L4/2</f>
+        <v>3.4895044170687166</v>
+      </c>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R4" s="1">
+        <f>I4</f>
+        <v>-12.541411560439439</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>-6.5158291380719096</v>
+      </c>
+      <c r="C5">
+        <v>9.5054135583592902</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <f>C3</f>
+        <v>-7.3708461838257655</v>
+      </c>
+      <c r="H5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5">
+        <f>F3*F7*F10+F5*F6*F9-F3*F9*F8-F4*F6*F10</f>
+        <v>-5.4171443685875715</v>
+      </c>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R5" s="1">
+        <f>-I5</f>
+        <v>5.4171443685875715</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <f>A4</f>
+        <v>-1.7283573982055174</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L6" s="1">
+        <f>-L4/2</f>
+        <v>-3.4895044170687166</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N6" s="1">
+        <f>L4*L4/4 + L3*L3*L3/27</f>
+        <v>-61.694800293432507</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <f>B4</f>
+        <v>-4.0710190005233819</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L7" s="1">
+        <f>L6</f>
+        <v>-3.4895044170687166</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N7" s="1">
+        <f>N6</f>
+        <v>-61.694800293432507</v>
+      </c>
+      <c r="O7" s="1" t="str">
+        <f>O6</f>
+        <v>)</v>
+      </c>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R7" s="1">
+        <f>-R3/3</f>
+        <v>-0.12423082326465895</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8">
+        <f>C4</f>
+        <v>6.9729152225895739</v>
+      </c>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9">
+        <f>B5</f>
+        <v>-6.5158291380719096</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L9" s="1" t="e">
+        <f>POWER(L6+SQRT(N6), 1/3)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R9" s="1">
+        <f>3*R7*R7+2*R3*R7+R4</f>
+        <v>-12.587711452786484</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10">
+        <f>C5</f>
+        <v>9.5054135583592902</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L10" s="1" t="e">
+        <f>POWER(L7-SQRT(N7), 1/3)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R10" s="1">
+        <f>R7*R7*R7+R3*R7*R7+R4*R7+R5</f>
+        <v>6.9790088341374332</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L12" s="1" t="e">
+        <f>L9+L10</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="R12" s="1" t="e">
+        <f>L12+R7</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1" t="e">
+        <f>L12*L12*L12+L3*L12+L4</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L16" s="1">
+        <f>SQRT(L6*L6+ABS(N6))</f>
+        <v>8.5948497002667015</v>
+      </c>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O16" s="1">
+        <f>SQRT(-L3/3)</f>
+        <v>2.048390543230342</v>
+      </c>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+    </row>
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="K17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L17" s="1">
+        <f>SQRT(-N6)/L6</f>
+        <v>-2.2509224306562285</v>
+      </c>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+    </row>
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="K18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L18" s="1">
+        <f>ATAN(L17)</f>
+        <v>-1.1527240986535725</v>
+      </c>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+    </row>
+    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="K19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L19" s="1">
+        <f>COS(L18/3)</f>
+        <v>0.92708307779626364</v>
+      </c>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+    </row>
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+    </row>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="K21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L21" s="1">
+        <f>2*O16*L19</f>
+        <v>3.7980564186934918</v>
+      </c>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+    </row>
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="K22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L22" s="1">
+        <f>SIGN(-L4/(L21*L21+L3))*ABS(L21)</f>
+        <v>-3.7980564186934918</v>
+      </c>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="R22" s="1">
+        <f>L22+R7</f>
+        <v>-3.9222872419581507</v>
+      </c>
+    </row>
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f>A3-R22</f>
+        <v>-1.8847997856717345</v>
+      </c>
+      <c r="B24">
+        <f t="shared" ref="B24:C24" si="0">B3</f>
+        <v>7.1044250520173655</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>-7.3708461838257655</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F24" s="1">
+        <f>SQRT(A24*A24+A25*A25)</f>
+        <v>2.5572816677088901</v>
+      </c>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1">
+        <f>F25</f>
+        <v>-0.7370325332056038</v>
+      </c>
+      <c r="I24" s="1">
+        <f>-F26</f>
+        <v>-0.67585726673353919</v>
+      </c>
+      <c r="J24" s="1">
+        <v>0</v>
+      </c>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1">
+        <f t="array" ref="L24:N26">MMULT(H24:J26,A24:C26)</f>
+        <v>2.5572816677088896</v>
+      </c>
+      <c r="M24" s="1">
+        <v>-5.1356709532373426</v>
+      </c>
+      <c r="N24" s="1">
+        <v>0.71985801122988402</v>
+      </c>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q24" s="1">
+        <f>SQRT(M25*M25+M26*M26)</f>
+        <v>8.1594049827397956</v>
+      </c>
+      <c r="R24" s="1"/>
+      <c r="S24" s="1">
+        <v>1</v>
+      </c>
+      <c r="T24" s="1">
+        <v>0</v>
+      </c>
+      <c r="U24" s="1">
+        <v>0</v>
+      </c>
+      <c r="V24" s="1"/>
+      <c r="W24" s="1">
+        <f t="array" ref="W24:Y26">MMULT(S24:U26,L24:N26)</f>
+        <v>2.5572816677088896</v>
+      </c>
+      <c r="X24" s="1">
+        <v>-5.1356709532373426</v>
+      </c>
+      <c r="Y24" s="1">
+        <v>0.71985801122988402</v>
+      </c>
+      <c r="Z24" s="1"/>
+      <c r="AA24" s="1">
+        <f t="array" ref="AA24:AC26">MMULT(W24:Y26,TRANSPOSE(H24:J26))</f>
+        <v>1.5861807476260861</v>
+      </c>
+      <c r="AB24" s="1">
+        <v>5.5135139705804734</v>
+      </c>
+      <c r="AC24" s="1">
+        <v>0.71985801122988402</v>
+      </c>
+      <c r="AE24" s="1">
+        <f t="array" ref="AE24:AG26">MMULT(AA24:AC26,TRANSPOSE(S24:U26))</f>
+        <v>1.5861807476260861</v>
+      </c>
+      <c r="AF24" s="1">
+        <v>2.7437642759616034</v>
+      </c>
+      <c r="AG24" s="1">
+        <v>4.8361957630016184</v>
+      </c>
+    </row>
+    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f t="shared" ref="A25:C26" si="1">A4</f>
+        <v>-1.7283573982055174</v>
+      </c>
+      <c r="B25">
+        <f>B4-R22</f>
+        <v>-0.14873175856523124</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="1"/>
+        <v>6.9729152225895739</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F25" s="1">
+        <f>A24/F24</f>
+        <v>-0.7370325332056038</v>
+      </c>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1">
+        <f>F26</f>
+        <v>0.67585726673353919</v>
+      </c>
+      <c r="I25" s="1">
+        <f>F25</f>
+        <v>-0.7370325332056038</v>
+      </c>
+      <c r="J25" s="1">
+        <v>0</v>
+      </c>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1">
+        <v>0</v>
+      </c>
+      <c r="M25" s="1">
+        <v>4.9111974421531954</v>
+      </c>
+      <c r="N25" s="1">
+        <v>-10.12090532564693</v>
+      </c>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q25" s="1">
+        <f>M25/Q24</f>
+        <v>0.60190632191222537</v>
+      </c>
+      <c r="R25" s="1"/>
+      <c r="S25" s="1">
+        <v>0</v>
+      </c>
+      <c r="T25" s="1">
+        <f>Q25</f>
+        <v>0.60190632191222537</v>
+      </c>
+      <c r="U25" s="1">
+        <f>-Q26</f>
+        <v>-0.79856670331419188</v>
+      </c>
+      <c r="V25" s="1"/>
+      <c r="W25" s="1">
+        <v>0</v>
+      </c>
+      <c r="X25" s="1">
+        <v>8.1594049827397956</v>
+      </c>
+      <c r="Y25" s="1">
+        <v>-16.814751660180832</v>
+      </c>
+      <c r="Z25" s="1"/>
+      <c r="AA25" s="1">
+        <v>-5.5145931498065384</v>
+      </c>
+      <c r="AB25" s="1">
+        <v>-6.0137469238791379</v>
+      </c>
+      <c r="AC25" s="1">
+        <v>-16.814751660180832</v>
+      </c>
+      <c r="AE25" s="1">
+        <v>-5.5145931498065384</v>
+      </c>
+      <c r="AF25" s="1">
+        <v>9.8079885084543914</v>
+      </c>
+      <c r="AG25" s="1">
+        <v>-14.923283381214956</v>
+      </c>
+    </row>
+    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="1"/>
+        <v>-6.5158291380719096</v>
+      </c>
+      <c r="C26">
+        <f>C5-R22</f>
+        <v>13.427700800317441</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F26" s="1">
+        <f>-A25/F24</f>
+        <v>0.67585726673353919</v>
+      </c>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1">
+        <v>0</v>
+      </c>
+      <c r="I26" s="1">
+        <v>0</v>
+      </c>
+      <c r="J26" s="1">
+        <v>1</v>
+      </c>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1">
+        <v>0</v>
+      </c>
+      <c r="M26" s="1">
+        <v>-6.5158291380719096</v>
+      </c>
+      <c r="N26" s="1">
+        <v>13.427700800317441</v>
+      </c>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q26" s="1">
+        <f>-M26/Q24</f>
+        <v>0.79856670331419188</v>
+      </c>
+      <c r="R26" s="1"/>
+      <c r="S26" s="1">
+        <v>0</v>
+      </c>
+      <c r="T26" s="1">
+        <f>Q26</f>
+        <v>0.79856670331419188</v>
+      </c>
+      <c r="U26" s="1">
+        <f>Q25</f>
+        <v>0.60190632191222537</v>
+      </c>
+      <c r="V26" s="1"/>
+      <c r="W26" s="1">
+        <v>0</v>
+      </c>
+      <c r="X26" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y26" s="1">
+        <v>-1.7763568394002505E-15</v>
+      </c>
+      <c r="Z26" s="1"/>
+      <c r="AA26" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB26" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC26" s="1">
+        <v>-1.7763568394002505E-15</v>
+      </c>
+      <c r="AE26" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF26" s="1">
+        <v>1.4185394251494754E-15</v>
+      </c>
+      <c r="AG26" s="1">
+        <v>-1.0692004116070304E-15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>3</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <f>AE24+R22</f>
+        <v>-2.3361064943320646</v>
+      </c>
+      <c r="B30">
+        <f t="shared" ref="B30:C31" si="2">AF24</f>
+        <v>2.7437642759616034</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="2"/>
+        <v>4.8361957630016184</v>
+      </c>
+    </row>
+    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <f t="shared" ref="A31:B32" si="3">AE25</f>
+        <v>-5.5145931498065384</v>
+      </c>
+      <c r="B31">
+        <f>AF25+R22</f>
+        <v>5.8857012664962411</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="2"/>
+        <v>-14.923283381214956</v>
+      </c>
+    </row>
+    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="3"/>
+        <v>1.4185394251494754E-15</v>
+      </c>
+      <c r="C32">
+        <f>AG26+R22</f>
+        <v>-3.9222872419581516</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:F8"/>
+      <selection activeCell="D5" sqref="D5:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2750,511 +4373,511 @@
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1">
         <f ca="1">RAND()*20-10</f>
-        <v>5.2707362700828693</v>
+        <v>-2.6728388852080931</v>
       </c>
       <c r="B1">
         <f t="shared" ref="B1:H15" ca="1" si="0">RAND()*20-10</f>
-        <v>7.8061503598087043</v>
+        <v>-1.8644607648761031</v>
       </c>
       <c r="C1">
         <f t="shared" ca="1" si="0"/>
-        <v>-7.6974523667497463</v>
+        <v>-1.7307927060859551</v>
       </c>
       <c r="D1">
         <f t="shared" ca="1" si="0"/>
-        <v>-4.409035232692748</v>
+        <v>-4.6870325668053159</v>
       </c>
       <c r="E1">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.6512608037293308</v>
+        <v>-2.7242401660702376</v>
       </c>
       <c r="F1">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.271009496516978</v>
+        <v>-4.6471324618948557</v>
       </c>
       <c r="G1">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.2833232714531668</v>
+        <v>7.6517233730537768</v>
       </c>
       <c r="H1">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.490404878541181</v>
+        <v>7.5793699183242111</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <f t="shared" ref="A2:A15" ca="1" si="1">RAND()*20-10</f>
-        <v>-3.9017032353913228</v>
+        <v>2.9001283224642229</v>
       </c>
       <c r="B2">
         <f t="shared" ca="1" si="0"/>
-        <v>-4.7498050474680964</v>
+        <v>6.3889775835658149</v>
       </c>
       <c r="C2">
         <f t="shared" ca="1" si="0"/>
-        <v>-9.5920456859887455</v>
+        <v>7.6365131419181935</v>
       </c>
       <c r="D2">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.7977159033701646</v>
+        <v>-4.8863287219868523</v>
       </c>
       <c r="E2">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.3478922854345399</v>
+        <v>9.769493863622948</v>
       </c>
       <c r="F2">
         <f t="shared" ca="1" si="0"/>
-        <v>6.9815923756412843</v>
+        <v>-5.9805742746655222</v>
       </c>
       <c r="G2">
         <f t="shared" ca="1" si="0"/>
-        <v>-8.6961514475755575</v>
+        <v>-9.0045378197709525</v>
       </c>
       <c r="H2">
         <f t="shared" ca="1" si="0"/>
-        <v>7.4470247398811438</v>
+        <v>2.4491104799447463</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.7926532928673371</v>
+        <v>-4.6788357096847939</v>
       </c>
       <c r="B3">
         <f t="shared" ca="1" si="0"/>
-        <v>-9.112838827033297</v>
+        <v>-8.0688821112563893</v>
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="0"/>
-        <v>6.129929943572904</v>
+        <v>1.4303486245145969</v>
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.84362077042376171</v>
+        <v>-5.159634806724589</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="0"/>
-        <v>-9.6262136633653821</v>
+        <v>2.6750183249399484</v>
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.4485474823604978</v>
+        <v>2.6075758252274621</v>
       </c>
       <c r="G3">
         <f t="shared" ca="1" si="0"/>
-        <v>7.0081706307484239</v>
+        <v>-3.1775249162456287</v>
       </c>
       <c r="H3">
         <f t="shared" ca="1" si="0"/>
-        <v>-9.142596913028127</v>
+        <v>-4.9528815972103519</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ca="1" si="1"/>
-        <v>-7.3155436335640793</v>
+        <v>-4.6070750429654472</v>
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>5.7358471028244331</v>
+        <v>8.035843748743833</v>
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.9706766723880467</v>
+        <v>8.8166079580971761</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="0"/>
-        <v>7.3839096266999782</v>
+        <v>7.021377601771146</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.689875081496556</v>
+        <v>-6.4533109515226954</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>1.0224321493223343</v>
+        <v>7.3895379923564803</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>8.3466764891595275</v>
+        <v>-6.4237878012139387</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.63527276823655221</v>
+        <v>3.3582668478289701</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" ca="1" si="1"/>
-        <v>0.92949001286098998</v>
+        <v>-3.8016944634513301</v>
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>-8.2768566413788811</v>
+        <v>1.7739534508410859</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>-9.0767203544499395</v>
+        <v>-2.5984614316325256</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.680184168523482</v>
+        <v>7.3691298350773948</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
-        <v>-8.478693007886573</v>
+        <v>2.8656915366524327</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>6.3657255683202543</v>
+        <v>-0.90861379041498225</v>
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="0"/>
-        <v>2.0641810794671223</v>
+        <v>6.8902107967208863</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.12652757480777055</v>
+        <v>7.3921407215884614</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" ca="1" si="1"/>
-        <v>9.5205418644688393</v>
+        <v>4.4661149712920807</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.35835814292275892</v>
+        <v>9.6173714617969672</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>7.3498545260518036</v>
+        <v>-7.936046131629519</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>7.9178783244758577</v>
+        <v>-3.391959050410005</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>-4.4840610189132279</v>
+        <v>-0.5645314429664765</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.0513413073557114</v>
+        <v>0.41685039099629329</v>
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="0"/>
-        <v>-4.5371387522183149</v>
+        <v>-8.5973779135630917</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.1483900222744463</v>
+        <v>-9.8912329108848951E-2</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" ca="1" si="1"/>
-        <v>3.7037177437765205</v>
+        <v>-3.1321140226008044</v>
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>0.40000958432014677</v>
+        <v>3.7890258963584316</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.34863670835447991</v>
+        <v>6.3231357028190445</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
-        <v>8.9844398016669906</v>
+        <v>-7.8945427764363751</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>3.4909154976289258</v>
+        <v>6.0252561896547796</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.7345733820041254</v>
+        <v>-3.9132473605596125</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="0"/>
-        <v>6.9025485095323944</v>
+        <v>7.8600062690711283</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="0"/>
-        <v>7.7390268904580068</v>
+        <v>-7.3415843100355982</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.7179139425521743</v>
+        <v>1.0091375253453663</v>
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.71875191773458269</v>
+        <v>-2.7235145461974604</v>
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>6.9302835436201562</v>
+        <v>6.0412776203892271</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.739482751155677</v>
+        <v>-3.5592173643348124</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.9787091000149104</v>
+        <v>1.7689810578103682</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>-9.3656031714214993</v>
+        <v>-0.79103890539632893</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.3408099405902609</v>
+        <v>1.3268151740147687</v>
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="0"/>
-        <v>6.1090930758783415</v>
+        <v>3.3072762238325009</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.471886896114917</v>
+        <v>-3.0637512761004926</v>
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>5.804495316583564</v>
+        <v>-8.4759876342276783</v>
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>5.7267585537736405</v>
+        <v>9.0743846746056747</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.1523442342536674</v>
+        <v>-5.9523367630237374</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.2717506757264649</v>
+        <v>8.1792678938118115</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.0971985064024388</v>
+        <v>-1.7082639029016242</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="0"/>
-        <v>6.5300063486196791</v>
+        <v>-5.2319921598482289</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="0"/>
-        <v>-7.5008140107747838</v>
+        <v>6.3056723861849164</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" ca="1" si="1"/>
-        <v>-7.224997718780366</v>
+        <v>-6.5162881564012416</v>
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>4.2173163001605616</v>
+        <v>-2.5999582834378803</v>
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>-4.93310692575192</v>
+        <v>9.7461862822713847</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="0"/>
-        <v>-8.0065176658303905</v>
+        <v>-1.7240795575514571</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="0"/>
-        <v>-8.0606155259817491</v>
+        <v>3.5876804955657491</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="0"/>
-        <v>4.4775291009610285</v>
+        <v>7.5160979205388507</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="0"/>
-        <v>-7.5169655309144767</v>
+        <v>-8.742617334241281</v>
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="0"/>
-        <v>2.1701457813537779</v>
+        <v>4.1134151371078271</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.3741583464695282</v>
+        <v>8.5683210563469387</v>
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2281345757029598</v>
+        <v>3.3395217148849525</v>
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="0"/>
-        <v>9.399433370477805</v>
+        <v>0.76272495251161132</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="0"/>
-        <v>7.2359817616122299</v>
+        <v>5.5120731441146162</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="0"/>
-        <v>-7.819085309099254</v>
+        <v>-4.4338218561096987</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.4596224000301046</v>
+        <v>4.4259037251420814</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="0"/>
-        <v>-9.9898664656287863</v>
+        <v>-0.41808942799394444</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="0"/>
-        <v>0.9239311506617387</v>
+        <v>1.5375642414756907</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" ca="1" si="1"/>
-        <v>8.6228835605115179</v>
+        <v>7.8229933308346276</v>
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>3.6230103750891196</v>
+        <v>0.1191552808532208</v>
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.3910218193491009</v>
+        <v>0.42066493064012711</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="0"/>
-        <v>5.178941480681063</v>
+        <v>9.2707572477893869</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="0"/>
-        <v>7.4166095942243757</v>
+        <v>-0.22426366311160706</v>
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="0"/>
-        <v>2.4267204720542033</v>
+        <v>-4.3727203626309885</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.10444082839700997</v>
+        <v>5.3164050406016035</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="0"/>
-        <v>5.1954378552265332</v>
+        <v>-9.8492705431683341</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" ca="1" si="1"/>
-        <v>9.9494553727826265</v>
+        <v>2.6729944665313159</v>
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>-8.7298946944446811</v>
+        <v>0.17626997690813084</v>
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="0"/>
-        <v>9.6307626312585768</v>
+        <v>3.3725730381796346</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.4106077254822793</v>
+        <v>-9.6874459487275644</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.5770937607708664</v>
+        <v>5.6890949974918783</v>
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="0"/>
-        <v>8.6442524176686248</v>
+        <v>-9.1453629802163476</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="0"/>
-        <v>1.5875480433999414</v>
+        <v>-0.59805071560499812</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.89163116539031861</v>
+        <v>-0.75475574704749349</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" ca="1" si="1"/>
-        <v>-7.5517442625100584</v>
+        <v>-0.79062280403412011</v>
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.15289921661264927</v>
+        <v>-2.5961784467493842</v>
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="0"/>
-        <v>8.5551754732605225</v>
+        <v>-9.2916013238857893</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="0"/>
-        <v>8.1090513332571845</v>
+        <v>-8.3222511514872437</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="0"/>
-        <v>-4.8233686241281841</v>
+        <v>-0.22325276269058669</v>
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.3181789539615405</v>
+        <v>-3.761581175877744</v>
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.3789347234729359</v>
+        <v>-1.4028668237668001</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="0"/>
-        <v>8.1992560294196331</v>
+        <v>-7.2169194363345373</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" ca="1" si="1"/>
-        <v>-8.3726640511431256</v>
+        <v>9.8993738877904498</v>
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>1.0832960560063682</v>
+        <v>3.3403404179875089</v>
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="0"/>
-        <v>-9.0945835813726035</v>
+        <v>8.7099528762286518</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="0"/>
-        <v>1.4576235933474369</v>
+        <v>-0.84522760217532422</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="0"/>
-        <v>5.0783016084891752</v>
+        <v>8.7916209939345968</v>
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.4848058484080475</v>
+        <v>-9.9498976400090875</v>
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.91305842104164192</v>
+        <v>3.9940845366359152</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.7737787495373976</v>
+        <v>6.5752181083960046</v>
       </c>
     </row>
   </sheetData>

</xml_diff>